<commit_message>
Site security Client Type - List, Create, Edit, Delete Client - List, Create, Edit, Delete
</commit_message>
<xml_diff>
--- a/Admin/Aroma Project Admin.xlsx
+++ b/Admin/Aroma Project Admin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sumary" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="Sub Task-Template" sheetId="6" r:id="rId6"/>
     <sheet name="Sub Task-Client" sheetId="7" r:id="rId7"/>
     <sheet name="Sub Task-Client Type" sheetId="8" r:id="rId8"/>
+    <sheet name="Sub Task-Security" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
   <si>
     <t>Developer</t>
   </si>
@@ -83,9 +84,6 @@
     <t>SMS - Not linked to anything        </t>
   </si>
   <si>
-    <t>Security        </t>
-  </si>
-  <si>
     <t>Reports        </t>
   </si>
   <si>
@@ -152,9 +150,6 @@
     <t>Sub Task-Template</t>
   </si>
   <si>
-    <t>Base obkect Identification</t>
-  </si>
-  <si>
     <t>Client Table design</t>
   </si>
   <si>
@@ -182,16 +177,46 @@
     <t>Clien Type data access models</t>
   </si>
   <si>
-    <t>Client Type list view and edit - Based on template to edit any standard lookup</t>
-  </si>
-  <si>
-    <t>Client Type display models - Based on template to display any standard lookup</t>
-  </si>
-  <si>
     <t>Sub Task-Client Type</t>
   </si>
   <si>
     <t>Update Git</t>
+  </si>
+  <si>
+    <t>Account Administration</t>
+  </si>
+  <si>
+    <t>Base object Identification</t>
+  </si>
+  <si>
+    <t>Unit Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client Type display models </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client Type list view and edit </t>
+  </si>
+  <si>
+    <t>Security Table design</t>
+  </si>
+  <si>
+    <t>Security data access models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security display models </t>
+  </si>
+  <si>
+    <t>Link user roles</t>
+  </si>
+  <si>
+    <t>Sub Task-Security</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Client Client type link</t>
   </si>
 </sst>
 </file>
@@ -624,7 +649,7 @@
       </c>
       <c r="C3">
         <f ca="1">SUM('Task List'!E:E)</f>
-        <v>1.75</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -633,7 +658,7 @@
       </c>
       <c r="C4" s="2">
         <f ca="1">SUM(C2:C3)</f>
-        <v>2.75</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -647,33 +672,33 @@
     <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2">
         <f ca="1">C6-C4</f>
-        <v>297.25</v>
+        <v>289.75</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="4">
         <f ca="1">SUM('Task List'!G:G)/Sumary!C10</f>
-        <v>1.7391304347826087E-2</v>
+        <v>0.10555555555555554</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <f ca="1">IF(E10&gt;F10,E10,F10)</f>
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="E10">
         <f>MAX('Task List'!A:A)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10">
         <f ca="1">SUM('Task List'!F:F)</f>
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -684,9 +709,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -710,13 +735,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -732,18 +757,18 @@
       </c>
       <c r="E2">
         <f ca="1">SUM(INDIRECT(CONCATENATE("'",I2,"'", "!D:D")))</f>
-        <v>1.75</v>
+        <v>1.25</v>
       </c>
       <c r="F2">
-        <f ca="1">SUM(INDIRECT(CONCATENATE("'",I2,"'", "!A:A")))</f>
-        <v>10</v>
+        <f ca="1">MAX(INDIRECT(CONCATENATE("'",I2,"'", "!A:A")))</f>
+        <v>4</v>
       </c>
       <c r="G2" s="4">
         <f ca="1">SUM(INDIRECT(CONCATENATE("'",I2,"'", "!E:E"))) /F2</f>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -762,15 +787,15 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F18" ca="1" si="2">SUM(INDIRECT(CONCATENATE("'",I3,"'", "!A:A")))</f>
+        <f ca="1">MAX(INDIRECT(CONCATENATE("'",I3,"'", "!A:A")))</f>
         <v>1</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" ref="G3:G18" ca="1" si="3">SUM(INDIRECT(CONCATENATE("'",I3,"'", "!E:E"))) /F3</f>
+        <f t="shared" ref="G3:G18" ca="1" si="2">SUM(INDIRECT(CONCATENATE("'",I3,"'", "!E:E"))) /F3</f>
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -786,18 +811,18 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F4">
+        <f ca="1">MAX(INDIRECT(CONCATENATE("'",I4,"'", "!A:A")))</f>
+        <v>2</v>
+      </c>
+      <c r="G4" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="G4" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -813,18 +838,18 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F5">
+        <f t="shared" ref="F5:F19" ca="1" si="3">MAX(INDIRECT(CONCATENATE("'",I5,"'", "!A:A")))</f>
+        <v>9</v>
+      </c>
+      <c r="G5" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="G5" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -840,18 +865,18 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F6">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G6" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="G6" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -870,15 +895,15 @@
         <v>0</v>
       </c>
       <c r="F7">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G7" s="4">
-        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -897,15 +922,15 @@
         <v>0</v>
       </c>
       <c r="F8">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G8" s="4">
-        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -924,15 +949,15 @@
         <v>0</v>
       </c>
       <c r="F9">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -951,15 +976,15 @@
         <v>0</v>
       </c>
       <c r="F10">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G10" s="4">
-        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -978,15 +1003,15 @@
         <v>0</v>
       </c>
       <c r="F11">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1005,15 +1030,15 @@
         <v>0</v>
       </c>
       <c r="F12">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G12" s="4">
-        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1032,23 +1057,23 @@
         <v>0</v>
       </c>
       <c r="F13">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G13" s="4">
-        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>20</v>
+      <c r="B14" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
@@ -1056,18 +1081,18 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G14" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G14" s="4">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I14" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1075,7 +1100,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
@@ -1086,15 +1111,15 @@
         <v>0</v>
       </c>
       <c r="F15">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G15" s="4">
-        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1102,7 +1127,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
@@ -1113,15 +1138,15 @@
         <v>0</v>
       </c>
       <c r="F16">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G16" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1129,7 +1154,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
@@ -1140,15 +1165,15 @@
         <v>0</v>
       </c>
       <c r="F17">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1156,7 +1181,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
@@ -1167,15 +1192,40 @@
         <v>0</v>
       </c>
       <c r="F18">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I18" t="s">
-        <v>42</v>
+        <v>1</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" ref="G19" ca="1" si="4">SUM(INDIRECT(CONCATENATE("'",I19,"'", "!E:E"))) /F19</f>
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1185,6 +1235,7 @@
     <hyperlink ref="B4" location="'Sub Task-Main Database'!A1" display="Main DB"/>
     <hyperlink ref="B5" location="'Sub Task-Client'!A1" display="Clients"/>
     <hyperlink ref="B6" location="'Sub Task-Client Type'!A1" display="Client Types"/>
+    <hyperlink ref="B14" location="'Sub Task-Security'!A1" display="Security        "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1205,10 +1256,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1217,7 +1268,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>0.25</v>
@@ -1239,10 +1290,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -1253,7 +1304,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="4">
         <v>0</v>
@@ -1264,7 +1315,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="4">
         <v>0</v>
@@ -1280,7 +1331,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,10 +1341,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1302,7 +1353,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1338,7 +1389,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,10 +1399,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1360,7 +1411,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1368,16 +1419,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1385,16 +1436,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1417,10 +1468,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1429,7 +1480,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1437,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1456,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,10 +1520,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1481,7 +1532,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1489,16 +1540,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E2" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1506,16 +1557,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E3" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1523,16 +1574,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E4" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1540,16 +1591,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E5" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1557,16 +1608,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E6" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1574,16 +1625,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E7" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1591,16 +1642,50 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E8" s="5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.25</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1610,11 +1695,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1623,10 +1706,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1635,7 +1718,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1643,16 +1726,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1660,16 +1743,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1677,16 +1760,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1694,16 +1777,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1711,7 +1794,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1721,6 +1804,160 @@
       </c>
       <c r="E6" s="5">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>